<commit_message>
allocation rule updated with 5 and 10 mi rad
</commit_message>
<xml_diff>
--- a/output/Allocation Rule/facility_data/allocation_rule_facility_demographics_1mi.xlsx
+++ b/output/Allocation Rule/facility_data/allocation_rule_facility_demographics_1mi.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -77,52 +77,106 @@
     <t xml:space="preserve">DECATUR</t>
   </si>
   <si>
+    <t xml:space="preserve">20.5752959055157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">142.549590220656</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHEMOURS EL DORADO</t>
   </si>
   <si>
     <t xml:space="preserve">EL DORADO</t>
   </si>
   <si>
+    <t xml:space="preserve">103.612502034919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45.6605130373706</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHEMOURS LOUISVILLE WORKS</t>
   </si>
   <si>
     <t xml:space="preserve">LOUISVILLE</t>
   </si>
   <si>
+    <t xml:space="preserve">36.0627684203524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166.099283620707</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iofina Chemical Inc.</t>
   </si>
   <si>
     <t xml:space="preserve">Covington</t>
   </si>
   <si>
+    <t xml:space="preserve">11.777227783969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1405.25430123102</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARKEMA, INC.</t>
   </si>
   <si>
     <t xml:space="preserve">CALVERT CITY</t>
   </si>
   <si>
+    <t xml:space="preserve">74.6569158825578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53.5114523922272</t>
+  </si>
+  <si>
     <t xml:space="preserve">HONEYWELL INTERNATIONAL INC - GEISMAR COMPLEX</t>
   </si>
   <si>
     <t xml:space="preserve">GEISMAR</t>
   </si>
   <si>
+    <t xml:space="preserve">120.261973778333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.7429777162124</t>
+  </si>
+  <si>
     <t xml:space="preserve">MEXICHEM FLUOR INC.</t>
   </si>
   <si>
     <t xml:space="preserve">SAINT GABRIEL</t>
   </si>
   <si>
+    <t xml:space="preserve">20.8371989696875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.5212447896903</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISLECHEM LLC</t>
   </si>
   <si>
     <t xml:space="preserve">GRAND ISLAND</t>
   </si>
   <si>
+    <t xml:space="preserve">17.2846381134759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">419.968295103647</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chemours - Corpus Christi Plant</t>
   </si>
   <si>
     <t xml:space="preserve">Gregory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130.239383628461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40.0646859239259</t>
   </si>
 </sst>
 </file>
@@ -526,14 +580,14 @@
       <c r="D2" t="n">
         <v>2</v>
       </c>
-      <c r="E2" t="n">
-        <v>20.5752959055157</v>
+      <c r="E2" t="s">
+        <v>21</v>
       </c>
       <c r="F2" t="n">
         <v>2933</v>
       </c>
-      <c r="G2" t="n">
-        <v>142.549590220656</v>
+      <c r="G2" t="s">
+        <v>22</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -566,18 +620,18 @@
         <v>15.239817639095</v>
       </c>
       <c r="R2" t="n">
-        <v>48.4768671804282</v>
+        <v>50</v>
       </c>
       <c r="S2" t="n">
-        <v>0.654347748196912</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
         <v>66990</v>
@@ -585,14 +639,14 @@
       <c r="D3" t="n">
         <v>3</v>
       </c>
-      <c r="E3" t="n">
-        <v>103.612502034919</v>
+      <c r="E3" t="s">
+        <v>25</v>
       </c>
       <c r="F3" t="n">
         <v>4731</v>
       </c>
-      <c r="G3" t="n">
-        <v>45.6605130373706</v>
+      <c r="G3" t="s">
+        <v>26</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -625,18 +679,18 @@
         <v>6.92743033168565</v>
       </c>
       <c r="R3" t="n">
-        <v>53.5633054085323</v>
+        <v>50</v>
       </c>
       <c r="S3" t="n">
-        <v>0.677420520359875</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
         <v>3707770</v>
@@ -644,14 +698,14 @@
       <c r="D4" t="n">
         <v>6</v>
       </c>
-      <c r="E4" t="n">
-        <v>36.0627684203524</v>
+      <c r="E4" t="s">
+        <v>29</v>
       </c>
       <c r="F4" t="n">
         <v>5990</v>
       </c>
-      <c r="G4" t="n">
-        <v>166.099283620707</v>
+      <c r="G4" t="s">
+        <v>30</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -684,31 +738,31 @@
         <v>12.0370280218545</v>
       </c>
       <c r="R4" t="n">
-        <v>36.1477352422131</v>
+        <v>30</v>
       </c>
       <c r="S4" t="n">
-        <v>0.458830595942571</v>
+        <v>0.366666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="n">
         <v>6</v>
       </c>
-      <c r="E5" t="n">
-        <v>11.777227783969</v>
+      <c r="E5" t="s">
+        <v>33</v>
       </c>
       <c r="F5" t="n">
         <v>16550</v>
       </c>
-      <c r="G5" t="n">
-        <v>1405.25430123102</v>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -741,18 +795,18 @@
         <v>2.97997206561507</v>
       </c>
       <c r="R5" t="n">
-        <v>29.842907243899</v>
+        <v>30</v>
       </c>
       <c r="S5" t="n">
-        <v>0.423111590275706</v>
+        <v>0.383333333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C6" t="n">
         <v>843010</v>
@@ -760,14 +814,14 @@
       <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="E6" t="n">
-        <v>74.6569158825578</v>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
       <c r="F6" t="n">
         <v>3995</v>
       </c>
-      <c r="G6" t="n">
-        <v>53.5114523922272</v>
+      <c r="G6" t="s">
+        <v>38</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -800,18 +854,18 @@
         <v>4.92117658956969</v>
       </c>
       <c r="R6" t="n">
-        <v>33.6375899227677</v>
+        <v>35</v>
       </c>
       <c r="S6" t="n">
-        <v>2.06644847650783</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C7" t="n">
         <v>413584</v>
@@ -819,14 +873,14 @@
       <c r="D7" t="n">
         <v>4</v>
       </c>
-      <c r="E7" t="n">
-        <v>120.261973778333</v>
+      <c r="E7" t="s">
+        <v>41</v>
       </c>
       <c r="F7" t="n">
         <v>9109</v>
       </c>
-      <c r="G7" t="n">
-        <v>75.7429777162124</v>
+      <c r="G7" t="s">
+        <v>42</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -859,18 +913,18 @@
         <v>3.76813326109933</v>
       </c>
       <c r="R7" t="n">
-        <v>113.583851851753</v>
+        <v>107.5</v>
       </c>
       <c r="S7" t="n">
-        <v>0.752476122065753</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C8" t="n">
         <v>18331</v>
@@ -878,14 +932,14 @@
       <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="n">
-        <v>20.8371989696875</v>
+      <c r="E8" t="s">
+        <v>45</v>
       </c>
       <c r="F8" t="n">
         <v>1657</v>
       </c>
-      <c r="G8" t="n">
-        <v>79.5212447896903</v>
+      <c r="G8" t="s">
+        <v>46</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -918,31 +972,31 @@
         <v>4.64695232347616</v>
       </c>
       <c r="R8" t="n">
-        <v>183.36971094438</v>
+        <v>200</v>
       </c>
       <c r="S8" t="n">
-        <v>0.942623213830884</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="n">
         <v>3</v>
       </c>
-      <c r="E9" t="n">
-        <v>17.2846381134759</v>
+      <c r="E9" t="s">
+        <v>49</v>
       </c>
       <c r="F9" t="n">
         <v>7259</v>
       </c>
-      <c r="G9" t="n">
-        <v>419.968295103647</v>
+      <c r="G9" t="s">
+        <v>50</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
@@ -975,18 +1029,18 @@
         <v>4.82075019391076</v>
       </c>
       <c r="R9" t="n">
-        <v>23.2706030556442</v>
+        <v>20</v>
       </c>
       <c r="S9" t="n">
-        <v>0.293287359108429</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C10" t="n">
         <v>17240</v>
@@ -994,14 +1048,14 @@
       <c r="D10" t="n">
         <v>3</v>
       </c>
-      <c r="E10" t="n">
-        <v>130.239383628461</v>
+      <c r="E10" t="s">
+        <v>53</v>
       </c>
       <c r="F10" t="n">
         <v>5218</v>
       </c>
-      <c r="G10" t="n">
-        <v>40.0646859239259</v>
+      <c r="G10" t="s">
+        <v>54</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1034,10 +1088,10 @@
         <v>0.709627924817798</v>
       </c>
       <c r="R10" t="n">
-        <v>17.8173659959865</v>
+        <v>20</v>
       </c>
       <c r="S10" t="n">
-        <v>0.214461191370049</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>